<commit_message>
Updated model with graph based approach and env variables
</commit_message>
<xml_diff>
--- a/output/future_state_estimates_dars.xlsx
+++ b/output/future_state_estimates_dars.xlsx
@@ -468,7 +468,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>This activity would take approximately 15 seconds because it involves a brief interaction similar to "Welcome and give application number" which takes 28.2143 seconds. However, "Welcome and get queue ticket" is likely simpler and faster as it doesn't involve assigning a unique application number, but rather just handing out a pre-printed queue ticket. Considering the technical infrastructure limitations and potential staff training needs, this time accounts for any minor delays or retries in the process.</t>
+          <t>This activity would take approximately 15 seconds because it involves a brief interaction similar to "Welcome and give application number," which took 28.2143 seconds. However, "Welcome and get queue ticket" is likely simpler and faster since it doesn't involve providing an application number, just issuing a ticket. Considering potential delays due to technical infrastructure limitations and the need for staff to be trained to efficiently handle the ticketing system, a slightly shorter time than the application number process is reasonable. Additionally, customer interaction time is minimal, as it involves just handing over a ticket.</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -488,7 +488,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Asking for verbal consent is a straightforward interaction similar to handing out documents or receiving them, which takes around 15 seconds. Considering the need for clear communication and potential customer queries, this activity might take slightly longer due to the necessity of ensuring customer understanding and agreement. Additionally, given the technical infrastructure and staff training levels in Ethiopia, there might be minor delays or the need for repetition to ensure clarity, but these should be minimal.</t>
+          <t>This activity would take approximately 15 seconds because it involves a brief verbal interaction similar to "Applicant hands out his/her documents" (15.1429 seconds). The process requires the customer service officer to ask for consent, which is a straightforward question, and the applicant to respond. Given the technical infrastructure limitations and potential need for clarification or repetition due to language barriers or understanding, this time accounts for minor delays or retries. Staff training would ensure that the request is communicated clearly and efficiently, minimizing the time required.</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -508,7 +508,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Requesting a FIN ID from the application is likely to involve accessing a digital system, similar to the CSO inputting the application number (33.5714 seconds) and checking personal data (48.7857 seconds). Considering the technical infrastructure limitations in Ethiopia, which may cause slower system responses, and the need for staff to be adequately trained to handle this specific request, additional time may be required. Customer interaction time is also a factor, as the applicant may need to provide or confirm information. Potential delays or retries due to system errors or incorrect data entry could further extend the time. Therefore, estimating 45 seconds for this activity is realistic.</t>
+          <t>Requesting a FIN ID from the application is similar to the activity where the CSO inputs the application number into the digital system, which takes 33.5714 seconds. Considering the technical infrastructure limitations in Ethiopia, there might be additional time required for system processing or connectivity issues. Staff training needs and potential customer interaction time could also add to the duration. Additionally, potential delays or retries due to system errors or incorrect data entry could extend the time. Therefore, a realistic estimate for this activity would be approximately 45 seconds.</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -528,11 +528,11 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Scanning a FIN QR code is a relatively quick process, similar to inputting an application number or taking a picture, which takes around 32 seconds. Considering the technical infrastructure in Ethiopia, there might be slight delays due to slower internet speeds or older scanning equipment. Staff may require some training to efficiently use the scanning devices, and there could be minor customer interaction to ensure the correct QR code is scanned. Additionally, potential retries if the scan fails initially could add a few extra seconds. Therefore, estimating around 30 seconds is realistic for this activity.</t>
+          <t>Scanning a FIN QR code is a relatively straightforward task, similar to inputting an application number or taking a picture, which takes around 32-33 seconds. However, considering the technical infrastructure limitations in Ethiopia, potential delays due to network issues, and the need for staff to be adequately trained to handle QR code scanning efficiently, an additional buffer time is necessary. Customer interaction time for explaining the process and potential retries if the scan fails initially also contribute to the estimated time. Therefore, a realistic processing time for scanning a FIN QR code would be approximately 45 seconds.</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>30</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6">
@@ -548,11 +548,11 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>This activity would take approximately 45 seconds because it involves orally gathering application data and entering it into the DARIS system. Similar activities, such as CSO checking and filling in personal data, take around 48.7857 seconds. Considering the technical infrastructure limitations in Ethiopia, staff may need additional time to ensure data accuracy. The need for customer interaction to clarify information and potential delays or retries due to system issues also contribute to the estimated time.</t>
+          <t>This activity would take approximately 65 seconds because it involves orally gathering information from the applicant and entering it into the DARIS system. Similar activities, such as filling in personal data and other information into the digital system, take 48.7857 and 93.0 seconds respectively. Considering the technical infrastructure limitations in Ethiopia, potential delays, and the need for staff to be adequately trained to handle oral data entry efficiently, a moderate time estimate is reasonable. Additionally, customer interaction time and the possibility of needing to repeat or clarify information contribute to this duration.</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>45</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7">
@@ -568,7 +568,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Printing the PA certificate can be compared to the activity of printing digital applications, which takes 77.7857 seconds. Given that the PA certificate might be a single document rather than multiple copies, the time could be slightly less. However, considering potential technical infrastructure limitations in Ethiopia, such as slower printing speeds or occasional printer malfunctions, and the need for staff to ensure the correct document is selected and printed, a realistic estimate would be around 65 seconds. This accounts for any minor delays or retries that might occur during the process.</t>
+          <t>This activity would take approximately 65 seconds because printing tasks such as "CSO prints digital application (3 copies)" take 77.7857 seconds, indicating that printing infrastructure might be slower due to technical limitations. The "Print PA certificate" might involve fewer copies or simpler documents, reducing time slightly. Staff training and customer interaction are minimal for printing, but potential delays or retries due to printer malfunctions or paper jams could occur, justifying a time estimate slightly lower than the digital application print time.</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -588,7 +588,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Stamping a PA certificate is similar to the existing activity of stamping documents, which takes 14.4286 seconds. Given the technical infrastructure and staff training in Ethiopia, the time required for stamping a PA certificate should be comparable. However, considering potential delays or retries due to customer interaction or equipment issues, an additional second is added to account for these factors, making it approximately 15 seconds.</t>
+          <t>Stamping a PA certificate is similar to the "Stamp documents" activity, which takes 14.4286 seconds. Given the technical infrastructure and staff training in Ethiopia, a slight increase in time might be necessary to account for potential delays or retries, especially if the certificate requires additional verification or handling. Therefore, estimating 15 seconds is realistic, considering the need for precision and possible customer interaction during the stamping process.</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -608,7 +608,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Signing a PA certificate is similar to the activity where the applicant signs on the 3 copies to confirm all data are correct, which takes 52.0714 seconds. Considering the PA certificate might be a single document, the signing process could be quicker. However, accounting for potential delays due to customer interaction, staff training needs, and possible retries if the signature is not clear, a realistic estimate would be around 45 seconds.</t>
+          <t>Signing a PA certificate is similar to the activity where the applicant signs on the 3 copies to confirm all data are correct, which takes 52.0714 seconds. Considering that the PA certificate might be a single document, the signing process could be quicker. However, taking into account potential delays due to customer interaction, staff guidance, and the need for accuracy, a realistic estimate would be slightly less than the time taken for signing multiple copies. Therefore, 45 seconds is a reasonable estimate, accounting for the technical infrastructure and staff training in Ethiopia.</t>
         </is>
       </c>
       <c r="D9" t="n">

</xml_diff>